<commit_message>
[enhancement] prepare for deployment
- add docker-compose.yml
- add .env file with default environment variables
- add sbt-native-packager
- add testData.xlsx - example file from which realty objects can be imported
- add default values to application.conf
</commit_message>
<xml_diff>
--- a/testData/testData.xlsx
+++ b/testData/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguen\Projects\scala\realty-value-calc\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070F7049-6E60-4AA8-9DE8-E68EA6D79296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1D6D54-59CD-46FE-8DF4-E21E03F77F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4200" yWindow="4200" windowWidth="28800" windowHeight="15345" xr2:uid="{B52F5C5C-200C-4E32-805F-552BA8D2DB8E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Местоположение</t>
   </si>
@@ -99,12 +99,6 @@
     <t>нет</t>
   </si>
   <si>
-    <t>балкон</t>
-  </si>
-  <si>
-    <t>лоджия</t>
-  </si>
-  <si>
     <t>без отделки</t>
   </si>
   <si>
@@ -112,6 +106,9 @@
   </si>
   <si>
     <t>современная отделка</t>
+  </si>
+  <si>
+    <t>есть</t>
   </si>
 </sst>
 </file>
@@ -512,7 +509,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,10 +584,10 @@
         <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="J2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K2">
         <v>500</v>
@@ -622,10 +619,10 @@
         <v>10</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="K3">
         <v>400</v>
@@ -657,10 +654,10 @@
         <v>5</v>
       </c>
       <c r="I4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K4">
         <v>100</v>

</xml_diff>